<commit_message>
Updated analyses, fixed miscoded cell
</commit_message>
<xml_diff>
--- a/Yuan et al (2022) raw data.xlsx
+++ b/Yuan et al (2022) raw data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pesavage/Documents/Research/Publications/Unpublished/Yuan et al (expansion of 2020 ISMIR for TISMIR)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pesavage/Documents/GitHub/music-copyright-expanded/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6932FAB0-4E58-254F-A4DA-6D77EEE88CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EBC9505-2697-A84E-A1C4-E8EB3AE5B648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="500" windowWidth="28800" windowHeight="16540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1093,11 +1093,13 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <u/>
@@ -1119,38 +1121,45 @@
       <sz val="12"/>
       <color theme="5"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="5"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <i/>
       <sz val="12"/>
       <color theme="5"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <i/>
       <sz val="12"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <i/>
       <sz val="12"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -1158,6 +1167,7 @@
       <sz val="12"/>
       <color theme="5"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1679,10 +1689,10 @@
   <dimension ref="A1:W48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="V34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D42" sqref="D42:D44"/>
+      <selection pane="bottomRight" activeCell="I16" sqref="I16:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2776,7 +2786,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>91</v>
       </c>
@@ -2801,11 +2811,11 @@
       <c r="H16" s="22">
         <v>14</v>
       </c>
-      <c r="I16" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="J16" s="21">
-        <v>1</v>
+      <c r="I16" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="J16" s="29">
+        <v>0</v>
       </c>
       <c r="K16" s="23" t="s">
         <v>330</v>

</xml_diff>